<commit_message>
DDL dos exercicios obrigatorios finalizados
</commit_message>
<xml_diff>
--- a/exercicios/1.2-exercicio-locadora/exe02-locadora-fisico.excel.xlsx
+++ b/exercicios/1.2-exercicio-locadora/exe02-locadora-fisico.excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105DF5E1-4FD7-4660-A866-33624EFEF643}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{105DF5E1-4FD7-4660-A866-33624EFEF643}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A3847FF6-7DBB-4C63-8A09-7C8C3676C37D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Veiculos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Nome</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>Localiza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -595,27 +601,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
     <col min="8" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>4</v>
       </c>
@@ -634,7 +640,7 @@
       <c r="L1" s="20"/>
       <c r="M1" s="20"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -669,7 +675,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -704,7 +710,7 @@
         <v>43485</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -739,7 +745,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D5" s="3">
         <v>3</v>
       </c>
@@ -768,7 +774,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D6" s="3">
         <v>4</v>
       </c>
@@ -797,7 +803,7 @@
         <v>43487</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>15</v>
       </c>
@@ -813,7 +819,7 @@
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -839,7 +845,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>1</v>
       </c>
@@ -865,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>2</v>
       </c>
@@ -891,7 +897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>3</v>
       </c>
@@ -906,6 +912,14 @@
       </c>
       <c r="J12" s="7">
         <v>3</v>
+      </c>
+      <c r="L12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>